<commit_message>
tomado de lista y comienzo de correcciones
</commit_message>
<xml_diff>
--- a/inasistencias-5b-Tec-Dig/alumnos-5b-Tec-Dig.xlsx
+++ b/inasistencias-5b-Tec-Dig/alumnos-5b-Tec-Dig.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -31,13 +31,16 @@
     <t xml:space="preserve">Dirección de correo</t>
   </si>
   <si>
-    <t xml:space="preserve">Gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Casas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcasas1972@gmail.com</t>
+    <t xml:space="preserve">Maitena Nontue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALDERETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mariano_c20031@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
   </si>
   <si>
     <t xml:space="preserve">Sofia Angelica</t>
@@ -49,6 +52,18 @@
     <t xml:space="preserve">alegresofiaangelica@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melody Berenice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALMARADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mabyvega74@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fabrizio Daniel</t>
   </si>
   <si>
@@ -67,6 +82,15 @@
     <t xml:space="preserve">lidiamax861@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Emilio Salvador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIANCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anamabel4020@yahoo.com.ar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tiziano</t>
   </si>
   <si>
@@ -85,6 +109,33 @@
     <t xml:space="preserve">alejodicerbo@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Tobías Baltazar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERNÁNDEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nataliafsalguero@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gonzalo Agustín</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOMEZ GONZALEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILGON71@YAHOO.COM.AR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dylan Ezequiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gutiérrez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dylangutierrez032@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maximo Iván</t>
   </si>
   <si>
@@ -94,6 +145,42 @@
     <t xml:space="preserve">maximolinares444@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Victoria Antonella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACIEL RUIZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vickymaciel2501@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cristian Gabriel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARTINEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">martinezbrisa2019@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facundo Nicolas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martorelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natalia.martorelli1984@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan Bautista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bautistamedina466@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Victoria Soledad</t>
   </si>
   <si>
@@ -103,6 +190,15 @@
     <t xml:space="preserve">miguez.madrid.victoria@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Matias Benjamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matute0201@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lautaro Nicolas</t>
   </si>
   <si>
@@ -112,6 +208,24 @@
     <t xml:space="preserve">ranlozo340@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Kevin Ezequiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEREZ DE ROSAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kevinperezderosas5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valentin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RÍOS PETRAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lucasrios1984@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Santiago Nahuel</t>
   </si>
   <si>
@@ -121,96 +235,6 @@
     <t xml:space="preserve">vanina.dolores.aguilar@hotmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Valentin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RÍOS PETRAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lucasrios1984@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melody Berenice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALMARADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mabyvega74@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emilio Salvador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIANCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anamabel4020@yahoo.com.ar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tobías Baltazar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERNÁNDEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nataliafsalguero@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dylan Ezequiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gutiérrez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dylangutierrez032@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denise Tamara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HERNANDEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denisetamarahernandez@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victoria Antonella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACIEL RUIZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vickymaciel2501@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cristian Gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARTINEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">martinezbrisa2019@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matias Benjamin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matute0201@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin Ezequiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEREZ DE ROSAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kevinperezderosas5@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Leon Agustin</t>
   </si>
   <si>
@@ -218,50 +242,15 @@
   </si>
   <si>
     <t xml:space="preserve">leonavilche@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maitena Nontue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALDERETE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mariano_c20031@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gonzalo Agustín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOMEZ GONZALEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SILGON71@YAHOO.COM.AR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facundo Nicolas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martorelli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natalia.martorelli1984@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juan Bautista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bautistamedina466@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -329,12 +318,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -347,6 +340,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF232629"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -355,13 +365,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -378,6 +388,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="n">
+        <v>45784</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -389,269 +402,322 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>77</v>
+      <c r="D25" s="0" t="n">
+        <f aca="false">COUNTIF(D2:D24,"p")</f>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion de asistencia y positivos
</commit_message>
<xml_diff>
--- a/inasistencias-5b-Tec-Dig/alumnos-5b-Tec-Dig.xlsx
+++ b/inasistencias-5b-Tec-Dig/alumnos-5b-Tec-Dig.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="310">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -1002,7 +1002,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1013,6 +1013,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC107"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -1057,7 +1063,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1086,15 +1092,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1107,7 +1117,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -1134,21 +1144,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF232629"/>
-          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1198,7 +1193,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFC107"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -1223,11 +1218,11 @@
   </sheetPr>
   <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AC21" activeCellId="0" sqref="AC21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -3340,17 +3335,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="9.39"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="9.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,6 +3392,9 @@
       <c r="N1" s="0" t="s">
         <v>94</v>
       </c>
+      <c r="O1" s="2" t="n">
+        <v>45856</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -3437,9 +3436,12 @@
       <c r="M2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="N2" s="8" t="n">
+      <c r="N2" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M2,L2,J2),0)</f>
         <v>7</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,7 +3460,7 @@
       <c r="E3" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="8" t="n">
         <v>7</v>
       </c>
       <c r="G3" s="2" t="n">
@@ -3485,9 +3487,12 @@
       <c r="M3" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N3" s="8" t="n">
+      <c r="N3" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M3,L3,J3),0)</f>
         <v>9</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3530,9 +3535,12 @@
       <c r="M4" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N4" s="8" t="n">
+      <c r="N4" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M4,L4,J4),0)</f>
         <v>10</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,9 +3583,12 @@
       <c r="M5" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N5" s="8" t="n">
+      <c r="N5" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M5,L5,J5),0)</f>
         <v>9</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3596,7 +3607,7 @@
       <c r="E6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="8" t="n">
         <v>7</v>
       </c>
       <c r="G6" s="2" t="n">
@@ -3623,9 +3634,12 @@
       <c r="M6" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N6" s="8" t="n">
+      <c r="N6" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M6,L6,J6),0)</f>
         <v>9</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,7 +3658,7 @@
       <c r="E7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="8" t="n">
         <v>7</v>
       </c>
       <c r="G7" s="2" t="n">
@@ -3671,9 +3685,12 @@
       <c r="M7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N7" s="8" t="n">
+      <c r="N7" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M7,L7,J7),0)</f>
         <v>9</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3692,19 +3709,22 @@
       <c r="E8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>1</v>
+      <c r="F8" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>45784</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">F8+H8/2</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J8" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(C8:E8,I8),0)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K8" s="7" t="str">
         <f aca="false">IF(J8&lt;7,"TEP","TEA")</f>
@@ -3716,9 +3736,12 @@
       <c r="M8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N8" s="8" t="n">
+      <c r="N8" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M8,L8,J8),0)</f>
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3761,9 +3784,12 @@
       <c r="M9" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N9" s="8" t="n">
+      <c r="N9" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M9,L9,J9),0)</f>
         <v>10</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,10 +3832,13 @@
       <c r="M10" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N10" s="8" t="n">
+      <c r="N10" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M10,L10,J10),0)</f>
         <v>8</v>
       </c>
+      <c r="O10" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -3827,23 +3856,26 @@
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>3</v>
+      <c r="F11" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>45856</v>
+      </c>
+      <c r="H11" s="9" t="n">
+        <v>23</v>
       </c>
       <c r="I11" s="0" t="n">
         <f aca="false">F11+H11/2</f>
-        <v>2.5</v>
+        <v>18.5</v>
       </c>
       <c r="J11" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(C11:E11,I11),0)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K11" s="7" t="str">
         <f aca="false">IF(J11&lt;7,"TEP","TEA")</f>
-        <v>TEP</v>
+        <v>TEA</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>4.5</v>
@@ -3851,9 +3883,12 @@
       <c r="M11" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N11" s="8" t="n">
+      <c r="N11" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M11,L11,J11),0)</f>
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3896,9 +3931,12 @@
       <c r="M12" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N12" s="8" t="n">
+      <c r="N12" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M12,L12,J12),0)</f>
         <v>9</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3917,7 +3955,7 @@
       <c r="E13" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F13" s="9" t="n">
+      <c r="F13" s="8" t="n">
         <v>5</v>
       </c>
       <c r="G13" s="2" t="n">
@@ -3944,9 +3982,12 @@
       <c r="M13" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N13" s="8" t="n">
+      <c r="N13" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M13,L13,J13),0)</f>
         <v>9</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3989,9 +4030,12 @@
       <c r="M14" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="N14" s="8" t="n">
+      <c r="N14" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M14,L14,J14),0)</f>
         <v>9</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4010,7 +4054,7 @@
       <c r="E15" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="8" t="n">
         <v>7</v>
       </c>
       <c r="G15" s="2" t="n">
@@ -4037,9 +4081,12 @@
       <c r="M15" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N15" s="8" t="n">
+      <c r="N15" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M15,L15,J15),0)</f>
         <v>9</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4082,9 +4129,12 @@
       <c r="M16" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="N16" s="8" t="n">
+      <c r="N16" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M16,L16,J16),0)</f>
         <v>7</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4127,9 +4177,12 @@
       <c r="M17" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N17" s="8" t="n">
+      <c r="N17" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M17,L17,J17),0)</f>
         <v>9</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4148,7 +4201,7 @@
       <c r="E18" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F18" s="9" t="n">
+      <c r="F18" s="8" t="n">
         <v>7</v>
       </c>
       <c r="G18" s="2" t="n">
@@ -4175,9 +4228,12 @@
       <c r="M18" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N18" s="8" t="n">
+      <c r="N18" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M18,L18,J18),0)</f>
         <v>8</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,9 +4276,12 @@
       <c r="M19" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N19" s="8" t="n">
+      <c r="N19" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M19,L19,J19),0)</f>
         <v>10</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4241,7 +4300,7 @@
       <c r="E20" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="F20" s="9" t="n">
+      <c r="F20" s="8" t="n">
         <v>8</v>
       </c>
       <c r="G20" s="2" t="n">
@@ -4268,9 +4327,12 @@
       <c r="M20" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="N20" s="8" t="n">
+      <c r="N20" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M20,L20,J20),0)</f>
         <v>8</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4313,9 +4375,12 @@
       <c r="M21" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N21" s="8" t="n">
+      <c r="N21" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M21,L21,J21),0)</f>
         <v>8</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,7 +4399,7 @@
       <c r="E22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="9" t="n">
+      <c r="F22" s="8" t="n">
         <v>6</v>
       </c>
       <c r="G22" s="2" t="n">
@@ -4361,9 +4426,12 @@
       <c r="M22" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="N22" s="8" t="n">
+      <c r="N22" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M22,L22,J22),0)</f>
         <v>8</v>
+      </c>
+      <c r="O22" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4406,9 +4474,12 @@
       <c r="M23" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="N23" s="8" t="n">
+      <c r="N23" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M23,L23,J23),0)</f>
         <v>7</v>
+      </c>
+      <c r="O23" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4451,24 +4522,28 @@
       <c r="M24" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="N24" s="8" t="n">
+      <c r="N24" s="6" t="n">
         <f aca="false">ROUND(AVERAGE(M24,L24,J24),0)</f>
         <v>8</v>
       </c>
+      <c r="O24" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O25" s="0" t="n">
+        <f aca="false">COUNTIF(O2:O24,"P")</f>
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J24">
-    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>7</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K2:K24">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"TEP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N24">
-    <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4489,11 +4564,11 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.9"/>
@@ -5098,11 +5173,11 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.25"/>
@@ -5602,11 +5677,11 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -6217,11 +6292,11 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -6705,11 +6780,11 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.64"/>
@@ -7129,11 +7204,11 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -7520,15 +7595,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.51"/>

</xml_diff>